<commit_message>
update RS ,add new SHOLDMAY config for Exchange 2019 and update  capture
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASHTTP/MS-ASHTTP_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASHTTP/MS-ASHTTP_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17CE8F7-FB6A-4085-A7C5-5398D29CC4D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91940EEE-4B59-4C93-9D81-F541E479526D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <definedName name="ScopeList">Requirements!#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -3641,9 +3642,6 @@
     <t>[In Appendix A: Product Behavior] Implementation can be configured to use different values for the allowed number of changes and the time period. (&lt;9&gt; Section 3.2.5.1.1:  Exchange 2013 , Exchange 2016, and Exchange 2019 can be configured to use different values for the allowed number of changes and the time period.)</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] Implementation can be configured to block clients for an amount of time other than 14 hours. (&lt;10&gt; Section 3.2.5.1.1:  Exchange 2013 and Exchange 2016 Preview can be configured to block clients for an amount of time other than 14 hours.)</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] Implementation does not return MS-ASProtocolVersions values of  16.1,16.0, 14.1 or 14.0. (&lt;11&gt; Section 3.2.5.2: Exchange 2007 SP1 does not return the value "16.1","16.0", "14.1", or "14.0" in the MS-ASProtocolVersions header.)</t>
   </si>
   <si>
@@ -3720,6 +3718,9 @@
   </si>
   <si>
     <t>[In Request headers]The authorization header is required. For more information on the authorization header requirements, see section 2.2.1.1.2.2.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation can be configured to block clients for an amount of time other than 14 hours. (&lt;10&gt; Section 3.2.5.1.1:  Exchange 2013, Exchange 2016, and Exchange 2019 can be configured to block clients for an amount of time other than 14 hours.)</t>
   </si>
 </sst>
 </file>
@@ -4055,6 +4056,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4078,21 +4094,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5199,128 +5200,128 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -5333,12 +5334,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -5351,12 +5352,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -5369,12 +5370,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -5387,60 +5388,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -14102,13 +14103,13 @@
     </row>
     <row r="365" spans="1:9" ht="30">
       <c r="A365" s="22" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B365" s="39" t="s">
         <v>850</v>
       </c>
       <c r="C365" s="20" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D365" s="38"/>
       <c r="E365" s="34" t="s">
@@ -14158,7 +14159,7 @@
         <v>1072</v>
       </c>
       <c r="C367" s="20" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D367" s="38"/>
       <c r="E367" s="34" t="s">
@@ -14183,7 +14184,7 @@
         <v>1072</v>
       </c>
       <c r="C368" s="20" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D368" s="38"/>
       <c r="E368" s="34" t="s">
@@ -14202,10 +14203,10 @@
     </row>
     <row r="369" spans="1:9">
       <c r="A369" s="22" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B369" s="24" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C369" s="20" t="s">
         <v>1073</v>
@@ -14227,13 +14228,13 @@
     </row>
     <row r="370" spans="1:9" ht="30">
       <c r="A370" s="22" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B370" s="24" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C370" s="20" t="s">
         <v>1092</v>
-      </c>
-      <c r="C370" s="20" t="s">
-        <v>1093</v>
       </c>
       <c r="D370" s="38"/>
       <c r="E370" s="34" t="s">
@@ -14252,13 +14253,13 @@
     </row>
     <row r="371" spans="1:9">
       <c r="A371" s="22" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B371" s="24" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C371" s="20" t="s">
         <v>1094</v>
-      </c>
-      <c r="C371" s="20" t="s">
-        <v>1095</v>
       </c>
       <c r="D371" s="38"/>
       <c r="E371" s="34" t="s">
@@ -14277,13 +14278,13 @@
     </row>
     <row r="372" spans="1:9" ht="30">
       <c r="A372" s="22" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B372" s="24" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C372" s="20" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D372" s="38"/>
       <c r="E372" s="34" t="s">
@@ -14302,13 +14303,13 @@
     </row>
     <row r="373" spans="1:9">
       <c r="A373" s="22" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B373" s="24" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C373" s="20" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D373" s="38"/>
       <c r="E373" s="22" t="s">
@@ -14327,13 +14328,13 @@
     </row>
     <row r="374" spans="1:9">
       <c r="A374" s="22" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B374" s="24" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C374" s="20" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D374" s="38"/>
       <c r="E374" s="22" t="s">
@@ -14727,13 +14728,13 @@
     </row>
     <row r="390" spans="1:9" ht="30">
       <c r="A390" s="22" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B390" s="24" t="s">
         <v>1104</v>
       </c>
-      <c r="B390" s="24" t="s">
+      <c r="C390" s="20" t="s">
         <v>1105</v>
-      </c>
-      <c r="C390" s="20" t="s">
-        <v>1106</v>
       </c>
       <c r="D390" s="38"/>
       <c r="E390" s="30" t="s">
@@ -17380,7 +17381,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="495" spans="1:9" ht="45">
+    <row r="495" spans="1:9" ht="60">
       <c r="A495" s="22" t="s">
         <v>422</v>
       </c>
@@ -17388,7 +17389,7 @@
         <v>484</v>
       </c>
       <c r="C495" s="20" t="s">
-        <v>1080</v>
+        <v>1106</v>
       </c>
       <c r="D495" s="30" t="s">
         <v>816</v>
@@ -17417,7 +17418,7 @@
         <v>484</v>
       </c>
       <c r="C496" s="20" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="D496" s="30" t="s">
         <v>817</v>
@@ -17446,7 +17447,7 @@
         <v>484</v>
       </c>
       <c r="C497" s="20" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D497" s="30" t="s">
         <v>817</v>
@@ -17473,7 +17474,7 @@
         <v>484</v>
       </c>
       <c r="C498" s="20" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="D498" s="30" t="s">
         <v>817</v>
@@ -17610,13 +17611,13 @@
     </row>
     <row r="503" spans="1:9" s="47" customFormat="1" ht="45.75" thickBot="1">
       <c r="A503" s="42" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B503" s="43">
         <v>6</v>
       </c>
       <c r="C503" s="44" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D503" s="45" t="s">
         <v>817</v>
@@ -17647,11 +17648,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -17659,6 +17655,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A463:H463 A405:I462 A464:I501 A20:I403">
@@ -17837,21 +17838,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -17900,10 +17886,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17923,16 +17931,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated RS and Code for MS-ASHTTP release 20240521
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASHTTP/MS-ASHTTP_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASHTTP/MS-ASHTTP_RequirementSpecification.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04B6716-3965-4B91-A729-2118A886248A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C9538E-089B-487A-B439-E2996C01AFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3625,9 +3625,6 @@
     <t>[In Appendix A: Product Behavior] &lt;6&gt; Section 3.1.5.2.3: The set time increases exponentially when multiple 503 errors are received.</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] Implementation does sometimes include a Retry-After header with HTTP 503 error responses. (&lt;7&gt; Section 3.2.5.1: Exchange 2010 and Exchange 2013 sometimes include a Retry-After header with HTTP 503 error responses.)</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] Implementation can be configured to track changes to the User-Agent header, but does not do so by default. (&lt;8&gt; Section 3.2.5.1:  Exchange 2013, Exchange 2016, and Exchange 2019 can be configured to track changes to the User-Agent header can be configured to track changes to the User-Agent header, but does not do so by default.)</t>
   </si>
   <si>
@@ -3719,6 +3716,9 @@
   </si>
   <si>
     <t xml:space="preserve">[In Device ID] The device ID is specified by the device-id-spec ABNF rule portion of the plain text query value. The device ID string MUST NOT contain commas or special characters. </t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation include a Retry-After header with HTTP 503 error responses. (&lt;7&gt; Section 3.2.5.1: Exchange 2010 and Exchange 2013 include a Retry-After header with HTTP 503 error responses.)</t>
   </si>
 </sst>
 </file>
@@ -4654,10 +4654,25 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I503" tableType="xml" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" connectionId="1">
-  <autoFilter ref="A19:I503" xr:uid="{00000000-0009-0000-0100-000001000000}">
+  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A19:I503" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="2.2.1.1.1.2.3"/>
+        <filter val="6"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <x14:filter val="[In Appendix A: Product Behavior] Implementation can be configured to block clients for an amount of time other than 14 hours. (&lt;10&gt; Section 3.2.5.1.1:  Exchange 2013, Exchange 2016, and Exchange 2019 can be configured to block clients for an amount of time other than 14 hours.)"/>
+            <x14:filter val="[In Appendix A: Product Behavior] Implementation can be configured to track changes to the User-Agent header, but does not do so by default. (&lt;8&gt; Section 3.2.5.1:  Exchange 2013, Exchange 2016, and Exchange 2019 can be configured to track changes to the User-Agent header can be configured to track changes to the User-Agent header, but does not do so by default.)"/>
+            <x14:filter val="[In Appendix A: Product Behavior] Implementation can be configured to use different values for the allowed number of changes and the time period. (&lt;9&gt; Section 3.2.5.1.1:  Exchange 2013 , Exchange 2016, and Exchange 2019 can be configured to use different values for the allowed number of changes and the time period.)"/>
+            <x14:filter val="[In Appendix A: Product Behavior] Implementation does sometimes include a Retry-After header with HTTP 503 error responses. (&lt;7&gt; Section 3.2.5.1: Exchange 2010 and Exchange 2013 sometimes include a Retry-After header with HTTP 503 error responses.)"/>
+          </mc:Choice>
+          <mc:Fallback>
+            <filter val="[In Appendix A: Product Behavior] Implementation does sometimes include a Retry-After header with HTTP 503 error responses. (&lt;7&gt; Section 3.2.5.1: Exchange 2010 and Exchange 2013 sometimes include a Retry-After header with HTTP 503 error responses.)"/>
+          </mc:Fallback>
+        </mc:AlternateContent>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4996,8 +5011,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J505"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C509" sqref="C509"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C491" sqref="C491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -5041,13 +5056,13 @@
         <v>25</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="9">
-        <v>45398</v>
+        <v>45433</v>
       </c>
       <c r="G3" s="22"/>
       <c r="J3" s="4"/>
@@ -8901,7 +8916,7 @@
       </c>
       <c r="I162" s="28"/>
     </row>
-    <row r="163" spans="1:9" ht="29">
+    <row r="163" spans="1:9" ht="29" hidden="1">
       <c r="A163" s="26" t="s">
         <v>184</v>
       </c>
@@ -8909,7 +8924,7 @@
         <v>441</v>
       </c>
       <c r="C163" s="17" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D163" s="26"/>
       <c r="E163" s="26" t="s">
@@ -8926,7 +8941,7 @@
       </c>
       <c r="I163" s="28"/>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" hidden="1">
       <c r="A164" s="26" t="s">
         <v>185</v>
       </c>
@@ -8951,7 +8966,7 @@
       </c>
       <c r="I164" s="28"/>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" hidden="1">
       <c r="A165" s="26" t="s">
         <v>186</v>
       </c>
@@ -8976,7 +8991,7 @@
       </c>
       <c r="I165" s="28"/>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" hidden="1">
       <c r="A166" s="26" t="s">
         <v>187</v>
       </c>
@@ -13955,13 +13970,13 @@
     </row>
     <row r="365" spans="1:9" ht="29" hidden="1">
       <c r="A365" s="18" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B365" s="35" t="s">
         <v>849</v>
       </c>
       <c r="C365" s="17" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D365" s="34"/>
       <c r="E365" s="30" t="s">
@@ -14011,7 +14026,7 @@
         <v>1070</v>
       </c>
       <c r="C367" s="17" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D367" s="34"/>
       <c r="E367" s="30" t="s">
@@ -14036,7 +14051,7 @@
         <v>1070</v>
       </c>
       <c r="C368" s="17" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D368" s="34"/>
       <c r="E368" s="30" t="s">
@@ -14055,10 +14070,10 @@
     </row>
     <row r="369" spans="1:9" hidden="1">
       <c r="A369" s="18" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B369" s="20" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C369" s="17" t="s">
         <v>1071</v>
@@ -14080,13 +14095,13 @@
     </row>
     <row r="370" spans="1:9" hidden="1">
       <c r="A370" s="18" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B370" s="20" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C370" s="17" t="s">
         <v>1089</v>
-      </c>
-      <c r="C370" s="17" t="s">
-        <v>1090</v>
       </c>
       <c r="D370" s="34"/>
       <c r="E370" s="30" t="s">
@@ -14105,13 +14120,13 @@
     </row>
     <row r="371" spans="1:9" hidden="1">
       <c r="A371" s="18" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B371" s="20" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C371" s="17" t="s">
         <v>1091</v>
-      </c>
-      <c r="C371" s="17" t="s">
-        <v>1092</v>
       </c>
       <c r="D371" s="34"/>
       <c r="E371" s="30" t="s">
@@ -14130,13 +14145,13 @@
     </row>
     <row r="372" spans="1:9" hidden="1">
       <c r="A372" s="18" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B372" s="20" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C372" s="17" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D372" s="34"/>
       <c r="E372" s="30" t="s">
@@ -14155,13 +14170,13 @@
     </row>
     <row r="373" spans="1:9" hidden="1">
       <c r="A373" s="18" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B373" s="20" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C373" s="17" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D373" s="34"/>
       <c r="E373" s="18" t="s">
@@ -14180,13 +14195,13 @@
     </row>
     <row r="374" spans="1:9" hidden="1">
       <c r="A374" s="18" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B374" s="20" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C374" s="17" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D374" s="34"/>
       <c r="E374" s="18" t="s">
@@ -14580,13 +14595,13 @@
     </row>
     <row r="390" spans="1:9" ht="29" hidden="1">
       <c r="A390" s="18" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B390" s="20" t="s">
         <v>1101</v>
       </c>
-      <c r="B390" s="20" t="s">
+      <c r="C390" s="17" t="s">
         <v>1102</v>
-      </c>
-      <c r="C390" s="17" t="s">
-        <v>1103</v>
       </c>
       <c r="D390" s="34"/>
       <c r="E390" s="26" t="s">
@@ -17127,7 +17142,7 @@
       </c>
       <c r="I490" s="28"/>
     </row>
-    <row r="491" spans="1:9" ht="43.5" hidden="1">
+    <row r="491" spans="1:9" ht="43.5">
       <c r="A491" s="26" t="s">
         <v>418</v>
       </c>
@@ -17135,7 +17150,7 @@
         <v>484</v>
       </c>
       <c r="C491" s="17" t="s">
-        <v>1075</v>
+        <v>1106</v>
       </c>
       <c r="D491" s="26"/>
       <c r="E491" s="26" t="s">
@@ -17177,7 +17192,7 @@
       </c>
       <c r="I492" s="28"/>
     </row>
-    <row r="493" spans="1:9" ht="58" hidden="1">
+    <row r="493" spans="1:9" ht="58">
       <c r="A493" s="26" t="s">
         <v>420</v>
       </c>
@@ -17185,7 +17200,7 @@
         <v>484</v>
       </c>
       <c r="C493" s="17" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="D493" s="26" t="s">
         <v>813</v>
@@ -17204,7 +17219,7 @@
       </c>
       <c r="I493" s="28"/>
     </row>
-    <row r="494" spans="1:9" ht="58" hidden="1">
+    <row r="494" spans="1:9" ht="58">
       <c r="A494" s="26" t="s">
         <v>421</v>
       </c>
@@ -17212,7 +17227,7 @@
         <v>484</v>
       </c>
       <c r="C494" s="17" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D494" s="26" t="s">
         <v>814</v>
@@ -17233,7 +17248,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="495" spans="1:9" ht="43.5" hidden="1">
+    <row r="495" spans="1:9" ht="43.5">
       <c r="A495" s="18" t="s">
         <v>422</v>
       </c>
@@ -17241,7 +17256,7 @@
         <v>484</v>
       </c>
       <c r="C495" s="17" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="D495" s="26" t="s">
         <v>815</v>
@@ -17270,7 +17285,7 @@
         <v>484</v>
       </c>
       <c r="C496" s="17" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D496" s="26" t="s">
         <v>816</v>
@@ -17299,7 +17314,7 @@
         <v>484</v>
       </c>
       <c r="C497" s="17" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D497" s="26" t="s">
         <v>816</v>
@@ -17326,7 +17341,7 @@
         <v>484</v>
       </c>
       <c r="C498" s="17" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D498" s="26" t="s">
         <v>816</v>
@@ -17463,13 +17478,13 @@
     </row>
     <row r="503" spans="1:9" s="43" customFormat="1" ht="44" hidden="1" thickBot="1">
       <c r="A503" s="38" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B503" s="39">
         <v>6</v>
       </c>
       <c r="C503" s="40" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D503" s="41" t="s">
         <v>816</v>
@@ -17513,31 +17528,31 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A404:G404 I404">
-    <cfRule type="expression" dxfId="17" priority="32">
+    <cfRule type="expression" dxfId="17" priority="31">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="31">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="15" priority="33">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="36">
+    <cfRule type="expression" dxfId="14" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="33">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:I403 A405:I462 A463:H463">
-    <cfRule type="expression" dxfId="13" priority="91">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="13" priority="45">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="47">
+    <cfRule type="expression" dxfId="12" priority="46">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="47">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="46">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="45">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="10" priority="91">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A464:I503">
@@ -17563,17 +17578,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H404">
-    <cfRule type="expression" dxfId="3" priority="27">
+    <cfRule type="expression" dxfId="3" priority="25">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="26">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="27">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="28">
+    <cfRule type="expression" dxfId="0" priority="28">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="25">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="26">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>